<commit_message>
Various fixes across the board.
- Comparison properly works again.
- Fixed mass import and the trinket removal.
- Fixed quests and their viewing so we know if they are raid, event or both.
- Fixed some issues with Guide quests and the new winter event.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Raids/raids.xlsx
+++ b/resources/data-imports/Raids/raids.xlsx
@@ -68,13 +68,13 @@
     <t>The Ice Queens Reign</t>
   </si>
   <si>
-    <t>She awoke in the in the middle of the night, with the snow falling down on her. She looked over, and saw the glass, the smells, the sights. She saw the blood, her husband, hanging upside down. She Screamed. “She never ascended from her own pain. She became trapped in her own memories. So much so that she is blind to her own son, who stands before her begging her to see him. But she never will.” “Now she rules a frozen waste land of memories and grief. She is the corruption of her own memories.”</t>
+    <t>She awoke in the middle of the night. The snow fell upon the ground as her eyes adjusted to the darkness. She could see that she was upside down. The SUV her and her husband were driving had lost control on the snow filled roads. She looked over to see her husband, also upside down – alas he was dead. That’s when it hit her, She was alone – completely and utterly alone. Her son committed suicide a year before, and now her husband was dead. “Hello there” comes a voice. She looks over to see feet, a moment later she is standing beside the man, wearing a fedora. “I am The Poet, You must be Isabella” the man states. “My son, Have you seen my son?” She asks. It was all she could mutter as the snow fell in the darkness of the night.</t>
   </si>
   <si>
     <t>The Ice Queen</t>
   </si>
   <si>
-    <t>Corrupted Ice Mage,Queens Knight of the Ice Rose,Lost Memory of Her Son,Haunting Snowman,Living Ice sickle ,Rabid Reindeer,Frozen King Krampus</t>
+    <t>Corrupted Ice Mage,Queens Knight of the Ice Rose,Lost Memory of Her Son,Haunting Snowman,Living Ice sickle,Rabid Reindeer,Frozen King Krampus</t>
   </si>
   <si>
     <t>Fathers Tomb</t>
@@ -435,9 +435,9 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="843.366" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="869.359" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="168.53" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="167.388" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="25.851" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="98.976" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="31.707" bestFit="true" customWidth="true" style="0"/>

</xml_diff>

<commit_message>
Finished the re-write of how we rebalance monsters
</commit_message>
<xml_diff>
--- a/resources/data-imports/Raids/raids.xlsx
+++ b/resources/data-imports/Raids/raids.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -23,6 +23,9 @@
     <t>story</t>
   </si>
   <si>
+    <t>raid_type</t>
+  </si>
+  <si>
     <t>raid_boss_id</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
     <t>Long before the merchants arrived at smugglers port, the place was run by pirates and escaped convicts. They kept the caves full of stolen goods, alcohol and gold. It wasn't until roughly around 100 years ago that the merchants had come through via the sea and waged a war with the smugglers and bandits of the area. There was a small period of peace with the bandits of the area for about 25 years, but it wasn't until recently when the merchants decided they wanted the port. The night the merchants came, was the night the moon was covered in blood. Now the son of a pirate lord who wonders the lands has come back to Smugglers Port to take back the port and other ports of the area. He is Rutheless and deadly.</t>
   </si>
   <si>
+    <t>pirate-lord</t>
+  </si>
+  <si>
     <t>Son of the Pirate Lords</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
     <t>She awoke in the middle of the night. The snow fell upon the ground as her eyes adjusted to the darkness. She could see that she was upside down. The SUV her and her husband were driving had lost control on the snow filled roads. She looked over to see her husband, also upside down – alas he was dead. That’s when it hit her, She was alone – completely and utterly alone. Her son committed suicide a year before, and now her husband was dead. “Hello there” comes a voice. She looks over to see feet, a moment later she is standing beside the man, wearing a fedora. “I am The Poet, You must be Isabella” the man states. “My son, Have you seen my son?” She asks. It was all she could mutter as the snow fell in the darkness of the night.</t>
   </si>
   <si>
+    <t>ice-queen</t>
+  </si>
+  <si>
     <t>The Ice Queen</t>
   </si>
   <si>
@@ -93,6 +102,9 @@
   </si>
   <si>
     <t>He is a Jester of Time. Given the power by his mother, stripped of his attachment to his brother. The world is a game that he plays in. The world is his toy, time is just a manipulation of that toy. With his lover dead, the hands of his soul are covered in blood.</t>
+  </si>
+  <si>
+    <t>jester-of-time</t>
   </si>
   <si>
     <t>Jester of Time</t>
@@ -450,7 +462,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,15 +472,16 @@
   <cols>
     <col min="1" max="1" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="869.359" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="208.663" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="25.851" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="98.976" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="31.707" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="47.131" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="208.663" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="98.976" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="47.131" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,83 +506,95 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated raid exports and raids
</commit_message>
<xml_diff>
--- a/resources/data-imports/Raids/raids.xlsx
+++ b/resources/data-imports/Raids/raids.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>name</t>
   </si>
@@ -38,6 +38,9 @@
     <t>corrupted_location_ids</t>
   </si>
   <si>
+    <t>scheduled_event_description</t>
+  </si>
+  <si>
     <t>item_specialty_reward_type</t>
   </si>
   <si>
@@ -92,6 +95,9 @@
     <t>Abandoned Village,Ice Dragons Port,Frozen Queens Bank,Fathers Tomb,The Frozen Wreck</t>
   </si>
   <si>
+    <t>Take part in a raid against the queen her self. She looks for her son, she grieves her husband. She is the queen of this realm and her suffering needs to end. Participate in The Ice Queens Reign Raid to earn a cosmetic item through the raid quests, and ancestral item for being the first to defeat her and a full set of Corrupted Ice gear (a more powerful set of gear!) for defeating her! All players are welcome to try their strength against her!</t>
+  </si>
+  <si>
     <t>Corrupted Ice</t>
   </si>
   <si>
@@ -134,13 +140,16 @@
     <t>frozen-king</t>
   </si>
   <si>
-    <t>Frozen Child of Fear,Corrupted Christmas Tree,Wailing Banshee of Ice,Bloody Snowman of rage,Faithless Prince of the Snow Garden,Zombified Cat of Yesterday,Faithless Priest of The Old Church</t>
+    <t>Faithless Priest of The Old Church,Zombified Cat of Yesterday,Faithless Prince of the Snow Garden,Bloody Snowman of rage,Wailing Banshee of Ice,Corrupted Christmas Tree,Frozen Child of Fear</t>
   </si>
   <si>
     <t>Forgotten Christmas Tree Lot</t>
   </si>
   <si>
     <t>Dilapidated House of the Drunk,Forgotten Christmas Tree Lot,Banshee Fields of Tomorrow,Ice Pirates Hideout</t>
+  </si>
+  <si>
+    <t>The king seeks his son, but he cries out for his wife. His is created of corrupted tears and failed magics. Take him down to earn an ancestral item (as the first person to kill him) and a full set of Corrupted Ice gear (a more powerful set of gear) as well! try your strength against him, regardless of your level!.</t>
   </si>
   <si>
     <t>Ancestral Soldiers Statue</t>
@@ -501,7 +510,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,11 +525,12 @@
     <col min="5" max="5" width="229.944" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="34.135" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="126.112" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="31.707" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="47.131" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="528.442" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="47.131" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,150 +558,159 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
         <v>16</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
       </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
+      <c r="J5" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="J6" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to raids and how events are scheduled.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Raids/raids.xlsx
+++ b/resources/data-imports/Raids/raids.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
@@ -125,6 +125,9 @@
     <t>Northren Port,Southren Port,Federation City</t>
   </si>
   <si>
+    <t>A crazed man filled with grief, pain and delsuional memories. Take down the Jester and get your self an ancestral item, an item of power. Bring peace to a corrupted land, or what little peace you can.</t>
+  </si>
+  <si>
     <t>Delusional Silver</t>
   </si>
   <si>
@@ -171,6 +174,9 @@
   </si>
   <si>
     <t>Federation Controlled Town,Northren Port,Southren Port,Federation City</t>
+  </si>
+  <si>
+    <t>The corrupted bishop has no love for those who he considers godless heathens. He will stomp you into oblivion and bring you befor ethe light of god to be judged. Take him down and earn an epic Ancestial Item!</t>
   </si>
 </sst>
 </file>
@@ -645,72 +651,78 @@
       <c r="G4" t="s">
         <v>35</v>
       </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
         <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to the raids and what ancestral items they drop
</commit_message>
<xml_diff>
--- a/resources/data-imports/Raids/raids.xlsx
+++ b/resources/data-imports/Raids/raids.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>The corrupted bishop has no love for those who he considers godless heathens. He will stomp you into oblivion and bring you befor ethe light of god to be judged. Take him down and earn an epic Ancestial Item!</t>
+  </si>
+  <si>
+    <t>Ancestral Fang of Delusional Thougts</t>
   </si>
 </sst>
 </file>
@@ -722,7 +725,7 @@
         <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>